<commit_message>
Actualizacion a mejor modelo
</commit_message>
<xml_diff>
--- a/Proyecto1/Data/SinEtiquetatest_cat_345_predictions.xlsx
+++ b/Proyecto1/Data/SinEtiquetatest_cat_345_predictions.xlsx
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160">
@@ -2312,7 +2312,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189">
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="288">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="295">
@@ -3592,7 +3592,7 @@
         </is>
       </c>
       <c r="B316" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="317">
@@ -4062,7 +4062,7 @@
         </is>
       </c>
       <c r="B363" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="364">
@@ -4112,7 +4112,7 @@
         </is>
       </c>
       <c r="B368" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="369">
@@ -4452,7 +4452,7 @@
         </is>
       </c>
       <c r="B402" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="403">
@@ -4502,7 +4502,7 @@
         </is>
       </c>
       <c r="B407" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="408">
@@ -4562,7 +4562,7 @@
         </is>
       </c>
       <c r="B413" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="414">
@@ -4702,7 +4702,7 @@
         </is>
       </c>
       <c r="B427" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="428">
@@ -5062,7 +5062,7 @@
         </is>
       </c>
       <c r="B463" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="464">
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="B475" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="476">
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="B479" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="480">
@@ -5462,7 +5462,7 @@
         </is>
       </c>
       <c r="B503" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="504">
@@ -5672,7 +5672,7 @@
         </is>
       </c>
       <c r="B524" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="525">
@@ -5952,7 +5952,7 @@
         </is>
       </c>
       <c r="B552" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="553">
@@ -6152,7 +6152,7 @@
         </is>
       </c>
       <c r="B572" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="573">
@@ -6682,7 +6682,7 @@
         </is>
       </c>
       <c r="B625" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="626">
@@ -6872,7 +6872,7 @@
         </is>
       </c>
       <c r="B644" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="645">
@@ -7002,7 +7002,7 @@
         </is>
       </c>
       <c r="B657" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="658">
@@ -7332,7 +7332,7 @@
         </is>
       </c>
       <c r="B690" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="691">
@@ -7712,7 +7712,7 @@
         </is>
       </c>
       <c r="B728" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="729">
@@ -9062,7 +9062,7 @@
         </is>
       </c>
       <c r="B863" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="864">
@@ -9112,7 +9112,7 @@
         </is>
       </c>
       <c r="B868" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="869">
@@ -9402,7 +9402,7 @@
         </is>
       </c>
       <c r="B897" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="898">
@@ -9472,7 +9472,7 @@
         </is>
       </c>
       <c r="B904" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="905">
@@ -10292,7 +10292,7 @@
         </is>
       </c>
       <c r="B986" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="987">
@@ -10602,7 +10602,7 @@
         </is>
       </c>
       <c r="B1017" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1018">
@@ -10832,7 +10832,7 @@
         </is>
       </c>
       <c r="B1040" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1041">
@@ -10892,7 +10892,7 @@
         </is>
       </c>
       <c r="B1046" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1047">
@@ -11392,7 +11392,7 @@
         </is>
       </c>
       <c r="B1096" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1097">
@@ -11802,7 +11802,7 @@
         </is>
       </c>
       <c r="B1137" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1138">
@@ -12262,7 +12262,7 @@
         </is>
       </c>
       <c r="B1183" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1184">
@@ -12272,7 +12272,7 @@
         </is>
       </c>
       <c r="B1184" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1185">
@@ -12322,7 +12322,7 @@
         </is>
       </c>
       <c r="B1189" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1190">
@@ -12342,7 +12342,7 @@
         </is>
       </c>
       <c r="B1191" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1192">
@@ -12522,7 +12522,7 @@
         </is>
       </c>
       <c r="B1209" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1210">
@@ -12562,7 +12562,7 @@
         </is>
       </c>
       <c r="B1213" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1214">
@@ -12982,7 +12982,7 @@
         </is>
       </c>
       <c r="B1255" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1256">
@@ -13542,7 +13542,7 @@
         </is>
       </c>
       <c r="B1311" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1312">
@@ -14072,7 +14072,7 @@
         </is>
       </c>
       <c r="B1364" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1365">
@@ -14102,7 +14102,7 @@
         </is>
       </c>
       <c r="B1367" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1368">
@@ -14152,7 +14152,7 @@
         </is>
       </c>
       <c r="B1372" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1373">
@@ -14262,7 +14262,7 @@
         </is>
       </c>
       <c r="B1383" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1384">
@@ -14472,7 +14472,7 @@
         </is>
       </c>
       <c r="B1404" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1405">
@@ -14592,7 +14592,7 @@
         </is>
       </c>
       <c r="B1416" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1417">
@@ -14632,7 +14632,7 @@
         </is>
       </c>
       <c r="B1420" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1421">
@@ -15382,7 +15382,7 @@
         </is>
       </c>
       <c r="B1495" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1496">
@@ -15562,7 +15562,7 @@
         </is>
       </c>
       <c r="B1513" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1514">
@@ -15662,7 +15662,7 @@
         </is>
       </c>
       <c r="B1523" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1524">
@@ -15782,7 +15782,7 @@
         </is>
       </c>
       <c r="B1535" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1536">
@@ -16232,7 +16232,7 @@
         </is>
       </c>
       <c r="B1580" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1581">
@@ -16922,7 +16922,7 @@
         </is>
       </c>
       <c r="B1649" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1650">
@@ -17182,7 +17182,7 @@
         </is>
       </c>
       <c r="B1675" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1676">
@@ -17412,7 +17412,7 @@
         </is>
       </c>
       <c r="B1698" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1699">
@@ -17742,7 +17742,7 @@
         </is>
       </c>
       <c r="B1731" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1732">
@@ -17762,7 +17762,7 @@
         </is>
       </c>
       <c r="B1733" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1734">
@@ -17972,7 +17972,7 @@
         </is>
       </c>
       <c r="B1754" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1755">

</xml_diff>